<commit_message>
chore: refactored factors to integers columns types
</commit_message>
<xml_diff>
--- a/dictionaries/example-dictionary/example-dictionary-non_rep.xlsx
+++ b/dictionaries/example-dictionary/example-dictionary-non_rep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sido/VisualStudioCodeProjects/ds-beta-dictionaries/dictionaries/example-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F423FF4C-8812-E945-981A-FCCD45722891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40AE92B-5F08-2B4E-8C11-138674CEE1D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="460" windowWidth="15960" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-32260" yWindow="-8940" windowWidth="15960" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -65,15 +65,6 @@
     <t>isMissing</t>
   </si>
   <si>
-    <t>gb</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>ne</t>
-  </si>
-  <si>
     <t>Netherlands</t>
   </si>
   <si>
@@ -86,10 +77,7 @@
     <t>Germany</t>
   </si>
   <si>
-    <t>ge</t>
-  </si>
-  <si>
-    <t>text</t>
+    <t>integer</t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:IP4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1622,7 +1610,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>8</v>
@@ -1644,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IU5"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1673,56 +1661,56 @@
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>16</v>
+      <c r="B2" s="3">
+        <v>0</v>
       </c>
       <c r="C2" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>14</v>
+      <c r="B3" s="3">
+        <v>1</v>
       </c>
       <c r="C3" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>21</v>
+      <c r="B4" s="3">
+        <v>2</v>
       </c>
       <c r="C4" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>15</v>
+      <c r="B5" s="3">
+        <v>3</v>
       </c>
       <c r="C5" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>